<commit_message>
added best results of ksom and cervCancer and VertebralColumn datasets
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_motorFailure_02_hold_01_best.xlsx
+++ b/results_analysis/ksom_motorFailure_02_hold_01_best.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98F49E7-5B79-4021-9F28-E45352D21F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA6E1E-3C1E-4852-A89B-EE7548E5C835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_hp_best" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,18 +463,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
@@ -549,6 +537,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,37 +549,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -927,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,7 +919,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -972,92 +951,188 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="C3" s="36">
+        <v>0.79605263157894701</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.86184210526315796</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.82894736842105299</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.84868421052631604</v>
+      </c>
+      <c r="I3" s="36">
+        <v>0.82894736842105299</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0.84868421052631604</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0.72368421052631604</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0.76973684210526305</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0.74342105263157898</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="38">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.82894736842105299</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.88815789473684204</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0.76973684210526305</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.84868421052631604</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0.84868421052631604</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="38">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.83552631578947401</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0.80263157894736903</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0.80263157894736903</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="J6" s="39">
+        <v>0.80263157894736903</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="45"/>
+      <c r="C7" s="38">
+        <v>0.78289473684210498</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0.80263157894736903</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.77631578947368396</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0.77631578947368396</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0.80921052631579005</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0.80263157894736903</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0.79605263157894701</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="40">
+        <v>0.82894736842105299</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.79605263157894701</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0.80263157894736903</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1067,118 +1142,118 @@
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36" t="s">
+      <c r="K11" s="34"/>
+      <c r="L11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="36" t="s">
+      <c r="M11" s="34"/>
+      <c r="N11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="38"/>
+      <c r="O11" s="35"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="25" t="s">
+      <c r="O12" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="22">
         <v>256</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="23">
         <v>512</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="23">
         <v>9.765625E-4</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="23">
         <v>512</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="23">
         <v>0.2</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="23">
         <v>8</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="23">
         <v>128</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="23">
         <v>2.6</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="23">
         <v>128</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="23">
         <v>3.125E-2</v>
       </c>
-      <c r="M13" s="27">
+      <c r="M13" s="23">
         <v>-4</v>
       </c>
-      <c r="N13" s="27">
+      <c r="N13" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="O13" s="4">
@@ -1186,229 +1261,229 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="24">
         <v>6.25E-2</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="25">
         <v>256</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>0.125</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="25">
         <v>256</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="25">
         <v>0.8</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="25">
         <v>128</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="25">
         <v>16</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="25">
         <v>0.6</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="25">
         <v>0.5</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="25">
         <v>6.25E-2</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="25">
         <v>-1</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="25">
         <v>1</v>
       </c>
-      <c r="O14" s="30">
+      <c r="O14" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="24">
         <v>4</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="25">
         <v>256</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="25">
         <v>3.90625E-3</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="25">
         <v>32</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="25">
         <v>0.2</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="25">
         <v>512</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="25">
         <v>512</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="25">
         <v>0.4</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="25">
         <v>256</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="25">
         <v>3.90625E-3</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="25">
         <v>-4</v>
       </c>
-      <c r="N15" s="29">
+      <c r="N15" s="25">
         <v>0.25</v>
       </c>
-      <c r="O15" s="30">
+      <c r="O15" s="26">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="24">
         <v>256</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="25">
         <v>512</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>9.765625E-4</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="25">
         <v>512</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="25">
         <v>0.2</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H16" s="25">
         <v>8</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="25">
         <v>4</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="25">
         <v>0.6</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="25">
         <v>128</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="25">
         <v>3.125E-2</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="25">
         <v>-1024</v>
       </c>
-      <c r="N16" s="29">
+      <c r="N16" s="25">
         <v>256</v>
       </c>
-      <c r="O16" s="30">
+      <c r="O16" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="24">
         <v>4</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="25">
         <v>512</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="25">
         <v>0.5</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="25">
         <v>16</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="25">
         <v>0.2</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="25">
         <v>4</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="25">
         <v>128</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="25">
         <v>0.4</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K17" s="25">
         <v>1</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="25">
         <v>0.5</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="25">
         <v>256</v>
       </c>
-      <c r="N17" s="29">
+      <c r="N17" s="25">
         <v>8</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="26">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="27">
         <v>4</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="28">
         <v>128</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="28">
         <v>1.5625E-2</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="28">
         <v>4</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="28">
         <v>2.4</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="28">
         <v>32</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="28">
         <v>512</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="28">
         <v>1</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="28">
         <v>512</v>
       </c>
-      <c r="L18" s="32">
+      <c r="L18" s="28">
         <v>6.25E-2</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="28">
         <v>-1024</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="28">
         <v>1024</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="29">
         <v>1024</v>
       </c>
     </row>
@@ -1420,6 +1495,7 @@
     <mergeCell ref="N11:O11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1427,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,7 +1516,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1472,92 +1548,188 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="49"/>
+      <c r="C3" s="36">
+        <v>0.73624999999999996</v>
+      </c>
+      <c r="D3" s="42">
+        <v>0.77756578947368404</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0.74434210526315803</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.73078947368421099</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.75565789473684197</v>
+      </c>
+      <c r="H3" s="30">
+        <v>0.76815789473684204</v>
+      </c>
+      <c r="I3" s="36">
+        <v>0.75256578947368402</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0.76111842105263205</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="15">
+        <v>0.69888157894736802</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.73875000000000002</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.71723684210526295</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0.664868421052632</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0.64460526315789501</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0.65901315789473702</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.67657894736842095</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0.65868421052631598</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="38">
+        <v>0.69585526315789503</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.75868421052631596</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.77868421052631598</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.66388157894736799</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0.70644736842105305</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0.73144736842105296</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.77401315789473701</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0.69750000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="15">
+        <v>0.73513157894736803</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.73453947368421002</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.72611842105263202</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.740592105263158</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0.73098684210526299</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0.73184210526315796</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.72690789473684203</v>
+      </c>
+      <c r="J6" s="39">
+        <v>0.73105263157894695</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="45"/>
+      <c r="C7" s="38">
+        <v>0.70302631578947405</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.71302631578947395</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.71151315789473701</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.62217105263157901</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0.70842105263157895</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0.70480263157894696</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0.70598684210526297</v>
+      </c>
+      <c r="J7" s="32">
+        <v>0.71506578947368404</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="40">
+        <v>0.69855263157894698</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.70019736842105296</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.69644736842105304</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.68559210526315795</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.70078947368421096</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0.70157894736842097</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0.70210526315789501</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.700921052631579</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1569,7 +1741,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1752,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1612,92 +1784,188 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="49"/>
+      <c r="C3" s="36">
+        <v>0.73355263157894701</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.77631578947368396</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0.74342105263157898</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.75657894736842102</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.76973684210526305</v>
+      </c>
+      <c r="I3" s="36">
+        <v>0.75657894736842102</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0.76315789473684204</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="38">
+        <v>0.69736842105263197</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0.74013157894736803</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0.71710526315789502</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0.66447368421052599</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0.65131578947368396</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0.66118421052631604</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.67763157894736903</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0.66447368421052599</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="38">
+        <v>0.69078947368421095</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.75657894736842102</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.78289473684210498</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.66118421052631604</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0.71052631578947401</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.77631578947368396</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0.69078947368421095</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="38">
+        <v>0.74342105263157898</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.72368421052631604</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0.74342105263157898</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.73355263157894701</v>
+      </c>
+      <c r="J6" s="39">
+        <v>0.73026315789473695</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
+      <c r="C7" s="38">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.71710526315789502</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0.71052631578947401</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.67105263157894701</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0.71052631578947401</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0.72039473684210498</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="40">
+        <v>0.69736842105263197</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.69078947368421095</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.69736842105263197</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.70723684210526305</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0.69736842105263197</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1720,7 +1988,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1752,92 +2020,188 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="35"/>
+      <c r="C3" s="36">
+        <v>0.79497889744593797</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.86048341273657103</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0.81565826707990796</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.822939068100358</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.82229919896081405</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.84211714763130596</v>
+      </c>
+      <c r="I3" s="36">
+        <v>0.82528735632183903</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0.84756921735338997</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
+      <c r="C4" s="38">
+        <v>0.79977288212582298</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0.80484225972120305</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0.787114845938375</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0.66521622347569198</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0.68028846153846201</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0.763334667912274</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.69612794612794604</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0.69790551903378695</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
+      <c r="C5" s="38">
+        <v>0.77838527428467297</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.827483848437227</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.88553709856035401</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.73121131741821399</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0.76682007451238199</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0.80820606535265205</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.84815184815184796</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0.84788756907279295</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
+      <c r="C6" s="38">
+        <v>0.81575757575757601</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.83344291036598706</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.806182121971596</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0.80733423663621695</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0.79090242112986098</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0.79463159791028704</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.81023720349563</v>
+      </c>
+      <c r="J6" s="39">
+        <v>0.79758522727272696</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
+      <c r="C7" s="38">
+        <v>0.76585912337207696</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.78500707213578502</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.74118589743589802</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0.77380952380952395</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0.792613502705246</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0.78631677600749805</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0.79281537176273997</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20"/>
+      <c r="C8" s="40">
+        <v>0.82293906810035899</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.78932778932778902</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.78943722943722905</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.788558511563207</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.79208401359043401</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.787114845938375</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0.80094290204295404</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1860,7 +2224,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1892,92 +2256,188 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="35"/>
+      <c r="C3" s="36">
+        <v>0.59840637168766198</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.74317303991916195</v>
+      </c>
+      <c r="E3" s="36">
+        <v>0.67996451767140498</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.65074292272818501</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.64523973524225497</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.69382112495271198</v>
+      </c>
+      <c r="I3" s="36">
+        <v>0.66980073678121599</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0.71203807176539202</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
+      <c r="C4" s="38">
+        <v>0.648214756713135</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0.67281118979944299</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0.602525754858379</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0.48894993513859802</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0.50973138706236398</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0.55209643889386495</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.52734261985938502</v>
+      </c>
+      <c r="J4" s="39">
+        <v>0.53052289814346898</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
+      <c r="C5" s="38">
+        <v>0.63640811632149796</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.67380299079472294</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.77758347563113195</v>
+      </c>
+      <c r="F5" s="38">
+        <v>0.47940052734087002</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0.53697039599737895</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0.619879676974465</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.69993217737882496</v>
+      </c>
+      <c r="J5" s="39">
+        <v>0.70478972665435802</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
+      <c r="C6" s="38">
+        <v>0.64980118437215195</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.67288580064924497</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.621094454832673</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0.61473957914402599</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0.58941587147857499</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0.61935734713022095</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.65062566476203298</v>
+      </c>
+      <c r="J6" s="39">
+        <v>0.61387082049830299</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
+      <c r="C7" s="38">
+        <v>0.61925828695198104</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.64450338663549001</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0.65133894727893005</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.58558657243888801</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0.55008085529054096</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0.655443838371221</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0.61918424760013901</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0.62387371800913405</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20"/>
+      <c r="C8" s="40">
+        <v>0.67679643823192404</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.585526427149756</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.57887445887445899</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.57821822211549501</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.57894736842105299</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.61609162039709997</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.57422969187675099</v>
+      </c>
+      <c r="J8" s="41">
+        <v>0.64349398368768995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>